<commit_message>
In the maps, use quintiles from CSV files, not our own calculations
</commit_message>
<xml_diff>
--- a/son/content/intermediate_outcomes/compulsory_school_age_(5_to_16_years)/attainment_at_age_16/2.0/IN13-2.0-attainment-at-age-16--by-ITL2-region-and-FSM--FSM-eligible--chart-format.xlsx
+++ b/son/content/intermediate_outcomes/compulsory_school_age_(5_to_16_years)/attainment_at_age_16/2.0/IN13-2.0-attainment-at-age-16--by-ITL2-region-and-FSM--FSM-eligible--chart-format.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Government Equality Hub\SON23\Code\smc-son\son\content\intermediate_outcomes\compulsory_school_age_(5_to_16_years)\attainment_at_age_16\2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE633AFA-769C-4D8C-A63C-77EABB377309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7852B9-C781-4D43-8716-91AEACC9316E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="29829" windowHeight="18000" xr2:uid="{9803E635-8E71-42B9-9F63-70E1FAD28722}"/>
   </bookViews>
@@ -18,12 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'IN13-2.0-attainment-at-age-16--'!$A$1:$U$255</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4352" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4353" uniqueCount="95">
   <si>
     <t>ind_code</t>
   </si>
@@ -305,6 +318,9 @@
   </si>
   <si>
     <t>West Yorkshire</t>
+  </si>
+  <si>
+    <t>Quintile_number</t>
   </si>
 </sst>
 </file>
@@ -1166,13 +1182,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC5DB49-23AE-421A-8BEC-A4B9D347B47D}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:U255"/>
+  <dimension ref="A1:V255"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1236,8 +1252,11 @@
       <c r="U1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1302,7 +1321,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -1367,7 +1386,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1432,7 +1451,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1497,7 +1516,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1562,7 +1581,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1627,7 +1646,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1692,7 +1711,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1757,7 +1776,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1822,7 +1841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1887,7 +1906,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1952,7 +1971,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2017,7 +2036,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -2082,7 +2101,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2147,7 +2166,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -12612,7 +12631,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="177" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A177" t="s">
         <v>21</v>
       </c>
@@ -12677,7 +12696,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="178" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A178" t="s">
         <v>21</v>
       </c>
@@ -12742,7 +12761,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="179" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A179" t="s">
         <v>21</v>
       </c>
@@ -12807,7 +12826,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="180" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A180" t="s">
         <v>21</v>
       </c>
@@ -12872,7 +12891,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="181" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A181" t="s">
         <v>21</v>
       </c>
@@ -12937,7 +12956,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="182" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A182" t="s">
         <v>21</v>
       </c>
@@ -13002,7 +13021,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="183" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A183" t="s">
         <v>21</v>
       </c>
@@ -13067,7 +13086,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="184" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A184" t="s">
         <v>21</v>
       </c>
@@ -13132,7 +13151,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="185" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A185" t="s">
         <v>21</v>
       </c>
@@ -13197,7 +13216,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="186" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A186" t="s">
         <v>21</v>
       </c>
@@ -13262,7 +13281,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="187" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A187" t="s">
         <v>21</v>
       </c>
@@ -13327,7 +13346,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="188" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A188" t="s">
         <v>21</v>
       </c>
@@ -13392,7 +13411,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="189" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A189" t="s">
         <v>21</v>
       </c>
@@ -13457,7 +13476,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="190" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A190" t="s">
         <v>21</v>
       </c>
@@ -13521,8 +13540,12 @@
       <c r="U190" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="191" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V190" t="str">
+        <f>MID(U190,2,1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="191" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A191" t="s">
         <v>21</v>
       </c>
@@ -13587,7 +13610,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="192" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A192" t="s">
         <v>21</v>
       </c>
@@ -13651,8 +13674,12 @@
       <c r="U192" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="193" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V192" t="str">
+        <f>MID(U192,2,1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="193" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A193" t="s">
         <v>21</v>
       </c>
@@ -13717,7 +13744,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="194" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A194" t="s">
         <v>21</v>
       </c>
@@ -13781,8 +13808,12 @@
       <c r="U194" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="195" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V194" t="str">
+        <f>MID(U194,2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A195" t="s">
         <v>21</v>
       </c>
@@ -13847,7 +13878,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="196" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A196" t="s">
         <v>21</v>
       </c>
@@ -13911,8 +13942,12 @@
       <c r="U196" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="197" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V196" t="str">
+        <f>MID(U196,2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A197" t="s">
         <v>21</v>
       </c>
@@ -13977,7 +14012,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="198" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A198" t="s">
         <v>21</v>
       </c>
@@ -14041,8 +14076,12 @@
       <c r="U198" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="199" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V198" t="str">
+        <f>MID(U198,2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A199" t="s">
         <v>21</v>
       </c>
@@ -14107,7 +14146,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="200" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A200" t="s">
         <v>21</v>
       </c>
@@ -14171,8 +14210,12 @@
       <c r="U200" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="201" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V200" t="str">
+        <f>MID(U200,2,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A201" t="s">
         <v>21</v>
       </c>
@@ -14237,7 +14280,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="202" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A202" t="s">
         <v>21</v>
       </c>
@@ -14301,8 +14344,12 @@
       <c r="U202" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="203" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V202" t="str">
+        <f>MID(U202,2,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A203" t="s">
         <v>21</v>
       </c>
@@ -14367,7 +14414,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="204" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A204" t="s">
         <v>21</v>
       </c>
@@ -14431,8 +14478,12 @@
       <c r="U204" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="205" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V204" t="str">
+        <f>MID(U204,2,1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A205" t="s">
         <v>21</v>
       </c>
@@ -14497,7 +14548,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="206" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A206" t="s">
         <v>21</v>
       </c>
@@ -14561,8 +14612,12 @@
       <c r="U206" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="207" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V206" t="str">
+        <f>MID(U206,2,1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A207" t="s">
         <v>21</v>
       </c>
@@ -14627,7 +14682,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="208" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A208" t="s">
         <v>21</v>
       </c>
@@ -14691,8 +14746,12 @@
       <c r="U208" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="209" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V208" t="str">
+        <f>MID(U208,2,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A209" t="s">
         <v>21</v>
       </c>
@@ -14757,7 +14816,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="210" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A210" t="s">
         <v>21</v>
       </c>
@@ -14821,8 +14880,12 @@
       <c r="U210" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="211" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V210" t="str">
+        <f>MID(U210,2,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A211" t="s">
         <v>21</v>
       </c>
@@ -14887,7 +14950,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="212" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A212" t="s">
         <v>21</v>
       </c>
@@ -14951,8 +15014,12 @@
       <c r="U212" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="213" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V212" t="str">
+        <f>MID(U212,2,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A213" t="s">
         <v>21</v>
       </c>
@@ -15017,7 +15084,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="214" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A214" t="s">
         <v>21</v>
       </c>
@@ -15081,8 +15148,12 @@
       <c r="U214" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="215" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V214" t="str">
+        <f>MID(U214,2,1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A215" t="s">
         <v>21</v>
       </c>
@@ -15147,7 +15218,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="216" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A216" t="s">
         <v>21</v>
       </c>
@@ -15211,8 +15282,12 @@
       <c r="U216" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="217" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V216" t="str">
+        <f>MID(U216,2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A217" t="s">
         <v>21</v>
       </c>
@@ -15277,7 +15352,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="218" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A218" t="s">
         <v>21</v>
       </c>
@@ -15341,8 +15416,12 @@
       <c r="U218" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="219" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V218" t="str">
+        <f>MID(U218,2,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A219" t="s">
         <v>21</v>
       </c>
@@ -15407,7 +15486,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="220" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A220" t="s">
         <v>21</v>
       </c>
@@ -15471,8 +15550,12 @@
       <c r="U220" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="221" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V220" t="str">
+        <f>MID(U220,2,1)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="221" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A221" t="s">
         <v>21</v>
       </c>
@@ -15537,7 +15620,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="222" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A222" t="s">
         <v>21</v>
       </c>
@@ -15601,8 +15684,12 @@
       <c r="U222" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="223" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V222" t="str">
+        <f>MID(U222,2,1)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="223" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A223" t="s">
         <v>21</v>
       </c>
@@ -15667,7 +15754,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="224" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A224" t="s">
         <v>21</v>
       </c>
@@ -15731,8 +15818,12 @@
       <c r="U224" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="225" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V224" t="str">
+        <f>MID(U224,2,1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="225" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A225" t="s">
         <v>21</v>
       </c>
@@ -15797,7 +15888,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="226" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A226" t="s">
         <v>21</v>
       </c>
@@ -15861,8 +15952,12 @@
       <c r="U226" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="227" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V226" t="str">
+        <f>MID(U226,2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A227" t="s">
         <v>21</v>
       </c>
@@ -15927,7 +16022,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="228" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A228" t="s">
         <v>21</v>
       </c>
@@ -15991,8 +16086,12 @@
       <c r="U228" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="229" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V228" t="str">
+        <f>MID(U228,2,1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A229" t="s">
         <v>21</v>
       </c>
@@ -16057,7 +16156,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="230" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="230" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A230" t="s">
         <v>21</v>
       </c>
@@ -16121,8 +16220,12 @@
       <c r="U230" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="231" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V230" t="str">
+        <f>MID(U230,2,1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A231" t="s">
         <v>21</v>
       </c>
@@ -16187,7 +16290,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="232" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A232" t="s">
         <v>21</v>
       </c>
@@ -16251,8 +16354,12 @@
       <c r="U232" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="233" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V232" t="str">
+        <f>MID(U232,2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A233" t="s">
         <v>21</v>
       </c>
@@ -16317,7 +16424,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="234" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A234" t="s">
         <v>21</v>
       </c>
@@ -16381,8 +16488,12 @@
       <c r="U234" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="235" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V234" t="str">
+        <f>MID(U234,2,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="235" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A235" t="s">
         <v>21</v>
       </c>
@@ -16447,7 +16558,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="236" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A236" t="s">
         <v>21</v>
       </c>
@@ -16511,8 +16622,12 @@
       <c r="U236" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="237" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V236" t="str">
+        <f>MID(U236,2,1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A237" t="s">
         <v>21</v>
       </c>
@@ -16577,7 +16692,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="238" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A238" t="s">
         <v>21</v>
       </c>
@@ -16641,8 +16756,12 @@
       <c r="U238" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="239" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V238" t="str">
+        <f>MID(U238,2,1)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="239" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A239" t="s">
         <v>21</v>
       </c>
@@ -16707,7 +16826,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="240" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A240" t="s">
         <v>21</v>
       </c>
@@ -16771,8 +16890,12 @@
       <c r="U240" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="241" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V240" t="str">
+        <f>MID(U240,2,1)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="241" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A241" t="s">
         <v>21</v>
       </c>
@@ -16837,7 +16960,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="242" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A242" t="s">
         <v>21</v>
       </c>
@@ -16901,8 +17024,12 @@
       <c r="U242" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="243" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V242" t="str">
+        <f>MID(U242,2,1)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="243" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A243" t="s">
         <v>21</v>
       </c>
@@ -16967,7 +17094,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="244" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A244" t="s">
         <v>21</v>
       </c>
@@ -17031,8 +17158,12 @@
       <c r="U244" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="245" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V244" t="str">
+        <f>MID(U244,2,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A245" t="s">
         <v>21</v>
       </c>
@@ -17097,7 +17228,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="246" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A246" t="s">
         <v>21</v>
       </c>
@@ -17161,8 +17292,12 @@
       <c r="U246" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="247" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V246" t="str">
+        <f>MID(U246,2,1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="247" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A247" t="s">
         <v>21</v>
       </c>
@@ -17227,7 +17362,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="248" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="248" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A248" t="s">
         <v>21</v>
       </c>
@@ -17291,8 +17426,12 @@
       <c r="U248" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="249" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V248" t="str">
+        <f>MID(U248,2,1)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="249" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A249" t="s">
         <v>21</v>
       </c>
@@ -17357,7 +17496,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="250" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="250" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A250" t="s">
         <v>21</v>
       </c>
@@ -17421,8 +17560,12 @@
       <c r="U250" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="251" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V250" t="str">
+        <f>MID(U250,2,1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="251" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A251" t="s">
         <v>21</v>
       </c>
@@ -17487,7 +17630,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="252" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A252" t="s">
         <v>21</v>
       </c>
@@ -17551,8 +17694,12 @@
       <c r="U252" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="253" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V252" t="str">
+        <f>MID(U252,2,1)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="253" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A253" t="s">
         <v>21</v>
       </c>
@@ -17617,7 +17764,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="254" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="254" spans="1:22" x14ac:dyDescent="0.4">
       <c r="A254" t="s">
         <v>21</v>
       </c>
@@ -17681,8 +17828,12 @@
       <c r="U254" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="255" spans="1:21" hidden="1" x14ac:dyDescent="0.4">
+      <c r="V254" t="str">
+        <f>MID(U254,2,1)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="255" spans="1:22" hidden="1" x14ac:dyDescent="0.4">
       <c r="A255" t="s">
         <v>21</v>
       </c>

</xml_diff>